<commit_message>
work on EDML count
</commit_message>
<xml_diff>
--- a/Holcene Revision Work/EDML LC/EDML-GICC Errors/New_Layers.xlsx
+++ b/Holcene Revision Work/EDML LC/EDML-GICC Errors/New_Layers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnmackay/Documents/GitHub/BICC/Holcene Revision Work/EDML LC/EDML-GICC Errors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4EF7C3-61FB-C843-B708-7AFEC37E3423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B5BAB4-FDE9-A44A-92A0-59E5E5193760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21820" yWindow="3420" windowWidth="34400" windowHeight="26700" xr2:uid="{4DA22EE9-F53B-0A41-9821-C6FC1BEF8675}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="26720" xr2:uid="{4DA22EE9-F53B-0A41-9821-C6FC1BEF8675}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -213,7 +213,7 @@
     <t>3551.5, 3557, 3559.5, 3567, 3458, 3401, 3431, 3418.5, 3442.5, 3459.5, 3465, 3468.5, 3484, 3487.5, 3498, 3515.5, 3525, 3526.5, 3534, 3541, 3543.5</t>
   </si>
   <si>
-    <t>128.8, 130.49, 140.48</t>
+    <t>128.8, 130.49, 140.44</t>
   </si>
 </sst>
 </file>
@@ -688,7 +688,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" zoomScaleNormal="167" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>